<commit_message>
C1: Add Driver_Settings sheet to example and test configs
- Added Driver_Settings sheet to examples/basic/catdriver_config.xlsx:
  - grade: ordinal type with D;C;B;A order, D as reference
  - campus: categorical
  - course_type: categorical
  - employment_field: categorical
  - All use missing_as_level strategy

- Recreated tests/test_data/test_config_binary.xlsx with Driver_Settings:
  - age_group: ordinal
  - income: ordinal
  - region: categorical

- Added scripts/add_driver_settings_sheet.R for future config updates

This completes patch C1: Example configs now include required Driver_Settings.
</commit_message>
<xml_diff>
--- a/modules/catdriver/examples/basic/catdriver_config.xlsx
+++ b/modules/catdriver/examples/basic/catdriver_config.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Settings" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Variables" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Driver_Settings" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,13 +27,23 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -47,8 +58,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -631,7 +645,6 @@
           <t>Campus Location</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -649,7 +662,6 @@
           <t>Course Type</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -667,7 +679,169 @@
           <t>Employment Field</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="19" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="19" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>driver</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>levels_order</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>reference_level</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>missing_strategy</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>rare_level_policy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ordinal</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>D;C;B;A</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>missing_as_level</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>warn_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>campus</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>categorical</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>missing_as_level</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>warn_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>course_type</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>categorical</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>missing_as_level</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>warn_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>employment_field</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>categorical</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>missing_as_level</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>warn_only</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>